<commit_message>
translation corrected and upgraded.
</commit_message>
<xml_diff>
--- a/ne/GuidelineInEnglishCumNepali.xlsx
+++ b/ne/GuidelineInEnglishCumNepali.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7396" uniqueCount="2577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7396" uniqueCount="2591">
   <si>
     <t>NVDA NVDA_VERSION User Guide</t>
   </si>
@@ -7710,9 +7710,6 @@
     <t>==== प्रणाली केन्द्रीयता पछ्याउ ====</t>
   </si>
   <si>
-    <t>पार्श्वचित्रको सिर्जना</t>
-  </si>
-  <si>
     <t>पार्श्वचित्रको सिर्जना गर्न नयाँ टाँकलाई दबाउनु होस् ।</t>
   </si>
   <si>
@@ -7747,6 +7744,51 @@
   </si>
   <si>
     <t xml:space="preserve"> - सन्झ्याल सर्बर  २००३ का लागि,  नेत्रवाणीलाई Service Pack 1 अथवा  पछिल्लो चाहिन्छ ।</t>
+  </si>
+  <si>
+    <t>+++ पार्श्वचित्रको सिर्जना +++</t>
+  </si>
+  <si>
+    <t>कुनै निश्चीत अनुप्रयोगमा गमन जस्ता उतेजकको प्रयोग  गरी यीनिहरूलाई स्वचालित रूपमा सक्रिय गर्न सकिन्छ ।</t>
+  </si>
+  <si>
+    <t>तपाइले   नेत्रवाणी मेनुमा रहेको  " पार्श्वचित्रको अभियोजन " लाई चयन गरी  पार्श्वचित्र अभियोजनको व्यबस्थापन गर्न सक्नु हुन्छ ।</t>
+  </si>
+  <si>
+    <t>तपाइले यो कार्य कुञ्जी आदेसको पर्योग गरेर पनि  गर्न सक्नु हुन्छ ।</t>
+  </si>
+  <si>
+    <t>- नेत्रवाणी + control+p: पार्श्वचित्र अभियोजन पातोलाई देखाउने छ ।</t>
+  </si>
+  <si>
+    <t>यो पातोको पहिलो नियन्त्रक भनेको पार्श्वचित्र सूची हो जहाँ बाट  तपाइले   उपलब्ध कुनै पनि पार्श्वचित्रलाई चयन गर्न सक्नु हुन्छ ।</t>
+  </si>
+  <si>
+    <t>वर्तमान  पार्स्वचित्र मानविय रूपले अथवा उतेजक द्वारा सक्रिय बनाइएका हुन् वा  सम्पादित हुदै छन् भन्ने जस्ता सक्रिय पार्श्वचित्र सम्बन्धी अतिरिक्त सुचनालाई पनि देखाइने छ।</t>
+  </si>
+  <si>
+    <t>यो पार्श्वचित्रलाई कसरी प्रयोग गर्ने भनेर तपाइले चयन गर्न सक्नु हुन्छ ।</t>
+  </si>
+  <si>
+    <t>+++ उतेजकहरू+++ [ConfigProfileTriggers]</t>
+  </si>
+  <si>
+    <t>+++ उतेजकहरूको अस्थाई निस्क्रियकरण +++</t>
+  </si>
+  <si>
+    <t>कहिले कहीं उतेजकहरूलाई अस्थाइ रुपमा निस्क्रिय गर्नु उपयोगी हुन्छ ।</t>
+  </si>
+  <si>
+    <t>उदाहरणका लागि,, तपाइले  कुनै मानविय रूपले सक्रिय पार्स्वचित्रलाई अथवा  तपाइको सामान्य अभियोजन लाइ उतेजक पार्श्वचित्रको हस्तक्षेप बिना नै सम्पादन गर्ने चाहना  राख्नु हुन्छ ।</t>
+  </si>
+  <si>
+    <t>तपाइले सबै उतेजकहरुलाई निस्क्रिय गर भन्ने  चेक बाकसमा टिक लगाएर यो कार्य गर्न सक्नु हुन्छ । the Temporarily disable all triggers checkbox in the Configuration Profiles dialog.</t>
+  </si>
+  <si>
+    <t>सबै पढ भन्ने पार्श्वचित्रको सम्पादन गर्न, तपाइले [मानविय रूपले सक्रिय गर #ConfigProfileManual] भन्ने पार्श्वचित्रलाई सक्रिय गर्नु पर्छ ।</t>
+  </si>
+  <si>
+    <t>अन्तमा, यदि मानविय रूपले वा उतेजक द्वारा सक्रिय गरिएको पार्श्वचित्र  छैन भने यो सामान्य अभियोजनको रूपमा  बचत हुनेछ ।</t>
   </si>
 </sst>
 </file>
@@ -7800,7 +7842,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="साधारण" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -7813,9 +7855,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="कार्यालय विषयवस्तु">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="कार्यालय">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -7853,7 +7895,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="कार्यालय">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -7925,7 +7967,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="कार्यालय">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -8101,8 +8143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1954"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="C1882" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C1882"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>
@@ -9210,10 +9252,10 @@
         <v>1055</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>2569</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>2570</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>2571</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>35</v>
@@ -9288,13 +9330,13 @@
         <v>1059</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>2573</v>
+        <v>2572</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>2575</v>
+        <v>2574</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>2573</v>
+        <v>2572</v>
       </c>
       <c r="E61" t="str">
         <f t="shared" ref="E61:E124" si="1">IF(B63=D61,C63,"")</f>
@@ -9309,13 +9351,13 @@
         <v>1060</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>2574</v>
+        <v>2573</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>2576</v>
+        <v>2575</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>2574</v>
+        <v>2573</v>
       </c>
       <c r="E62" t="str">
         <f t="shared" si="1"/>
@@ -29932,7 +29974,7 @@
         <v>2381</v>
       </c>
       <c r="C1113" s="2" t="s">
-        <v>2381</v>
+        <v>2577</v>
       </c>
       <c r="D1113" s="2" t="s">
         <v>2381</v>
@@ -29980,7 +30022,7 @@
         <v>2383</v>
       </c>
       <c r="C1116" s="2" t="s">
-        <v>2383</v>
+        <v>2578</v>
       </c>
       <c r="D1116" s="2" t="s">
         <v>2383</v>
@@ -29998,7 +30040,7 @@
         <v>2384</v>
       </c>
       <c r="C1117" s="2" t="s">
-        <v>2384</v>
+        <v>2579</v>
       </c>
       <c r="D1117" s="2" t="s">
         <v>2384</v>
@@ -30034,7 +30076,7 @@
         <v>2434</v>
       </c>
       <c r="C1119" s="2" t="s">
-        <v>2434</v>
+        <v>2580</v>
       </c>
       <c r="D1119" s="2" t="s">
         <v>2434</v>
@@ -30103,7 +30145,7 @@
         <v>2385</v>
       </c>
       <c r="C1123" s="2" t="s">
-        <v>2385</v>
+        <v>2581</v>
       </c>
       <c r="D1123" s="2" t="s">
         <v>2385</v>
@@ -30121,7 +30163,7 @@
         <v>2386</v>
       </c>
       <c r="C1124" s="2" t="s">
-        <v>2569</v>
+        <v>2568</v>
       </c>
       <c r="D1124" s="2" t="s">
         <v>2386</v>
@@ -30142,7 +30184,7 @@
         <v>2387</v>
       </c>
       <c r="C1125" s="2" t="s">
-        <v>2387</v>
+        <v>2582</v>
       </c>
       <c r="D1125" s="2" t="s">
         <v>2387</v>
@@ -30175,7 +30217,7 @@
         <v>2388</v>
       </c>
       <c r="C1127" s="2" t="s">
-        <v>2568</v>
+        <v>2567</v>
       </c>
       <c r="D1127" s="2" t="s">
         <v>2388</v>
@@ -30208,7 +30250,7 @@
         <v>2389</v>
       </c>
       <c r="C1129" s="2" t="s">
-        <v>2567</v>
+        <v>2566</v>
       </c>
       <c r="D1129" s="2" t="s">
         <v>2389</v>
@@ -30238,7 +30280,7 @@
         <v>2390</v>
       </c>
       <c r="C1131" s="2" t="s">
-        <v>2564</v>
+        <v>2576</v>
       </c>
       <c r="D1131" s="2" t="s">
         <v>2390</v>
@@ -30259,7 +30301,7 @@
         <v>2391</v>
       </c>
       <c r="C1132" s="2" t="s">
-        <v>2565</v>
+        <v>2564</v>
       </c>
       <c r="D1132" s="2" t="s">
         <v>2391</v>
@@ -30289,7 +30331,7 @@
         <v>2392</v>
       </c>
       <c r="C1134" s="2" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="D1134" s="2" t="s">
         <v>2392</v>
@@ -30307,7 +30349,7 @@
         <v>2393</v>
       </c>
       <c r="C1135" s="2" t="s">
-        <v>2393</v>
+        <v>2583</v>
       </c>
       <c r="D1135" s="2" t="s">
         <v>2393</v>
@@ -30586,7 +30628,7 @@
         <v>2406</v>
       </c>
       <c r="C1151" s="2" t="s">
-        <v>2406</v>
+        <v>2584</v>
       </c>
       <c r="D1151" s="2" t="s">
         <v>2406</v>
@@ -30883,7 +30925,7 @@
         <v>2416</v>
       </c>
       <c r="C1168" s="2" t="s">
-        <v>2416</v>
+        <v>2590</v>
       </c>
       <c r="D1168" s="2" t="s">
         <v>2416</v>
@@ -30916,7 +30958,7 @@
         <v>2417</v>
       </c>
       <c r="C1170" s="2" t="s">
-        <v>2417</v>
+        <v>2589</v>
       </c>
       <c r="D1170" s="2" t="s">
         <v>2417</v>
@@ -30946,7 +30988,7 @@
         <v>2418</v>
       </c>
       <c r="C1172" s="2" t="s">
-        <v>2418</v>
+        <v>2585</v>
       </c>
       <c r="D1172" s="2" t="s">
         <v>2418</v>
@@ -30964,7 +31006,7 @@
         <v>2419</v>
       </c>
       <c r="C1173" s="2" t="s">
-        <v>2419</v>
+        <v>2586</v>
       </c>
       <c r="D1173" s="2" t="s">
         <v>2419</v>
@@ -30982,7 +31024,7 @@
         <v>2420</v>
       </c>
       <c r="C1174" s="2" t="s">
-        <v>2420</v>
+        <v>2587</v>
       </c>
       <c r="D1174" s="2" t="s">
         <v>2420</v>
@@ -31003,7 +31045,7 @@
         <v>2421</v>
       </c>
       <c r="C1175" s="2" t="s">
-        <v>2421</v>
+        <v>2588</v>
       </c>
       <c r="D1175" s="2" t="s">
         <v>2421</v>
@@ -44634,7 +44676,7 @@
       <c r="B1853" s="2"/>
       <c r="C1853" s="2"/>
       <c r="E1853" t="str">
-        <f t="shared" ref="E1853:E1916" si="29">IF(B1855=D1853,C1855,"")</f>
+        <f t="shared" ref="E1853:E1880" si="29">IF(B1855=D1853,C1855,"")</f>
         <v/>
       </c>
       <c r="F1853" s="1" t="s">
@@ -45068,7 +45110,7 @@
         <v>2494</v>
       </c>
       <c r="D1876" s="1" t="s">
-        <v>2572</v>
+        <v>2571</v>
       </c>
       <c r="E1876" t="str">
         <f t="shared" si="29"/>

</xml_diff>

<commit_message>
upgraded to 9811 and deleted old versions.
</commit_message>
<xml_diff>
--- a/ne/GuidelineInEnglishCumNepali.xlsx
+++ b/ne/GuidelineInEnglishCumNepali.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7396" uniqueCount="2591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7396" uniqueCount="2597">
   <si>
     <t>NVDA NVDA_VERSION User Guide</t>
   </si>
@@ -7789,6 +7789,24 @@
   </si>
   <si>
     <t>अन्तमा, यदि मानविय रूपले वा उतेजक द्वारा सक्रिय गरिएको पार्श्वचित्र  छैन भने यो सामान्य अभियोजनको रूपमा  बचत हुनेछ ।</t>
+  </si>
+  <si>
+    <t>यदि तपाइ यो पार्श्वचित्रलाई मानविय रूपमा मात्र चलाउन चाहनु हुन्छ भने, मानविय सक्रियतालाई चयनगर्नु होला, जो पुर्व निर्धारित गरिएको छ ।</t>
+  </si>
+  <si>
+    <t>अन्यथा, उतेजकलाई चयन गर्नु होस्, जसले यो पार्स्वचित्रलाई स्वचालित रुपमा सक्रिय गरोस् ।</t>
+  </si>
+  <si>
+    <t>सजिलै  बुझ्नका लागि, यदि तपाइले यो पार्श्वचित्रको नाम प्रविष्टि गर्नु भएको छैन भने, उतेजकलाई चयन गर्दा उक्त नामलाई चढाउँने छ ।</t>
+  </si>
+  <si>
+    <t>उतेजक सम्बन्धी थप जानकारीका लागि  [तलको #ConfigProfileTriggers] हेर्नु होला ।</t>
+  </si>
+  <si>
+    <t>'ठीक' टाँकलाई दबाउँदा  पार्श्वचित्रको सिर्जना गर्ने छ र  यसलाई सम्पादन गर्न सकियोस् भनेर उक्त पार्श्वचित्रको अभियोजन  पातोलाई बन्द गर्ने छ ।</t>
+  </si>
+  <si>
+    <t>+++ मानविय सक्रियता +++[ConfigProfileManual]</t>
   </si>
 </sst>
 </file>
@@ -8143,8 +8161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1954"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1882" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C1882"/>
+    <sheetView tabSelected="1" topLeftCell="A1141" workbookViewId="0">
+      <selection activeCell="B1143" sqref="B1143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="25.5" x14ac:dyDescent="0.7"/>
@@ -30367,7 +30385,7 @@
         <v>2394</v>
       </c>
       <c r="C1136" s="2" t="s">
-        <v>2394</v>
+        <v>2591</v>
       </c>
       <c r="D1136" s="2" t="s">
         <v>2394</v>
@@ -30385,7 +30403,7 @@
         <v>2395</v>
       </c>
       <c r="C1137" s="2" t="s">
-        <v>2395</v>
+        <v>2592</v>
       </c>
       <c r="D1137" s="2" t="s">
         <v>2395</v>
@@ -30403,7 +30421,7 @@
         <v>2396</v>
       </c>
       <c r="C1138" s="2" t="s">
-        <v>2396</v>
+        <v>2593</v>
       </c>
       <c r="D1138" s="2" t="s">
         <v>2396</v>
@@ -30424,7 +30442,7 @@
         <v>2397</v>
       </c>
       <c r="C1139" s="2" t="s">
-        <v>2397</v>
+        <v>2594</v>
       </c>
       <c r="D1139" s="2" t="s">
         <v>2397</v>
@@ -30457,7 +30475,7 @@
         <v>2398</v>
       </c>
       <c r="C1141" s="2" t="s">
-        <v>2398</v>
+        <v>2595</v>
       </c>
       <c r="D1141" s="2" t="s">
         <v>2398</v>
@@ -30484,7 +30502,7 @@
         <v>2141</v>
       </c>
       <c r="B1143" s="2" t="s">
-        <v>2399</v>
+        <v>2596</v>
       </c>
       <c r="C1143" s="2" t="s">
         <v>2399</v>

</xml_diff>

<commit_message>
re-committed to replace the self-made binary one.
</commit_message>
<xml_diff>
--- a/ne/GuidelineInEnglishCumNepali.xlsx
+++ b/ne/GuidelineInEnglishCumNepali.xlsx
@@ -8394,8 +8394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1936"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A1926" workbookViewId="0">
+      <selection activeCell="A1933" sqref="A1933"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>